<commit_message>
network visualizations ME 52, 21
</commit_message>
<xml_diff>
--- a/output/module_DEG_DML_PSGE_overlap_results_15May2019.xlsx
+++ b/output/module_DEG_DML_PSGE_overlap_results_15May2019.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rong\Box Sync\Projects\Intragenomic Conflict\WGCNA_Intragenomic_Conflict\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{16849D2D-C0D7-4349-A56C-9E6DCDCC25C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E8EFF9E0-F762-408B-8DD6-E223449AD3BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="module_DEG_DML_PSGE_overlap_res" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Summary" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="module_DEG_DML_PSGE_overlap_res" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="129">
   <si>
     <t>module_name</t>
   </si>
@@ -290,9 +291,6 @@
     <t>Module Size</t>
   </si>
   <si>
-    <t>Overlaps</t>
-  </si>
-  <si>
     <t>All DML,DEG,PSGE</t>
   </si>
   <si>
@@ -351,6 +349,66 @@
   </si>
   <si>
     <t>N_sig_overlap_cats</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Ovary Correlation</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>KEGGs</t>
+  </si>
+  <si>
+    <t>mRNA surveillance pathway</t>
+  </si>
+  <si>
+    <t>FoxO signaling pathway</t>
+  </si>
+  <si>
+    <t>Endocytosis</t>
+  </si>
+  <si>
+    <t>mTOR signaling pathway</t>
+  </si>
+  <si>
+    <t>Apoptosis - fly</t>
+  </si>
+  <si>
+    <t>Notch signaling pathway</t>
+  </si>
+  <si>
+    <t>Hippo signaling pathway - fly</t>
+  </si>
+  <si>
+    <t>Hippo signaling pathway - multiple species</t>
+  </si>
+  <si>
+    <t>Metabolic pathways</t>
+  </si>
+  <si>
+    <t>Mitophagy - animal</t>
+  </si>
+  <si>
+    <t>MAPK signaling pathway - fly</t>
+  </si>
+  <si>
+    <t>Neuroactive ligand-receptor interaction</t>
+  </si>
+  <si>
+    <t>Spliceosome</t>
+  </si>
+  <si>
+    <t>Protein processing in endoplasmic reticulum</t>
+  </si>
+  <si>
+    <t>Pentose phosphate pathway</t>
   </si>
 </sst>
 </file>
@@ -692,7 +750,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -822,6 +880,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -867,9 +938,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -883,6 +955,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1317,13 +1392,2010 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
+    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="6">
+        <v>49</v>
+      </c>
+      <c r="C3" s="7">
+        <v>3.0727421786891403E-5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4.1408677795375499E-2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.31240589928971E-5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.5519218270286801E-3</v>
+      </c>
+      <c r="G3" s="6">
+        <v>5.1642273572096702E-3</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2.4966587012933399E-3</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3.9374514759771299E-10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3">
+        <f>COUNTIF(C3:I3, "&lt;.05")</f>
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6">
+        <v>170</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3.82764266623059E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.1596458589716801E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>9.1145456733761995E-2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.189328930289766</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3.0580940643272201E-3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>4.8680620812544498E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <v>4.1400693470308697E-2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4">
+        <f>COUNTIF(C4:I4, "&lt;.05")</f>
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6">
+        <v>113</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.00917630888977E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3.2636679075339799E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.28736385326993102</v>
+      </c>
+      <c r="F5" s="6">
+        <v>9.8320086435050205E-2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.48127789556697198</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4.2980989788245001E-2</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.25808089613206397</v>
+      </c>
+      <c r="J5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5">
+        <f>COUNTIF(C5:I5, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>110</v>
+      </c>
+      <c r="M5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6">
+        <v>97</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3.5842824028819401E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>8.2715555596224498E-4</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.25222148564160102</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.36689888451437702</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.40408191903381802</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.66227001630235E-2</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.10749916758988599</v>
+      </c>
+      <c r="J6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6">
+        <f>COUNTIF(C6:I6, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1210</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2.0028910919589501E-4</v>
+      </c>
+      <c r="D7" s="6">
+        <v>4.4746813663012501E-3</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.14778188417742599</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.33807821000114202</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.56393306759295503</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.66049254676589397</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7">
+        <f>COUNTIF(C7:I7, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" t="s">
+        <v>115</v>
+      </c>
+      <c r="O7" t="s">
+        <v>116</v>
+      </c>
+      <c r="P7" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>118</v>
+      </c>
+      <c r="R7" t="s">
+        <v>119</v>
+      </c>
+      <c r="S7" t="s">
+        <v>120</v>
+      </c>
+      <c r="T7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6">
+        <v>63</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.37650756713623701</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.25991936329413001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.5110016556087799E-2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3.5159386902263702E-2</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.596454664061291</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.52261680978378</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1.3409651500317901E-8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8">
+        <f>COUNTIF(C8:I8, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="6">
+        <v>80</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.119810503657902</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.71879934460762096</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2.36831800814752E-2</v>
+      </c>
+      <c r="F9" s="6">
+        <v>6.2428503719827999E-3</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.106283581417212</v>
+      </c>
+      <c r="H9" s="6">
+        <v>6.6532792544706995E-2</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1.3999679440974699E-3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9">
+        <f>COUNTIF(C9:I9, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>109</v>
+      </c>
+      <c r="M9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="6">
+        <v>39</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.25337999817992202</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.124610014084039</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.110074023491538</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1.43307083179275E-2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.7944823064988499E-2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.06057084232558E-3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.38626838697876198</v>
+      </c>
+      <c r="J10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10">
+        <f>COUNTIF(C10:I10, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="6">
+        <v>97</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.51725204957717397</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.785452385130046</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.25222148564160102</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.36689888451437702</v>
+      </c>
+      <c r="G11" s="6">
+        <v>4.7136880600406899E-4</v>
+      </c>
+      <c r="H11" s="6">
+        <v>9.3785787513489495E-4</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5.6903370904137798E-12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11">
+        <f>COUNTIF(C11:I11, "&lt;.05")</f>
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4.5505193561934396E-3</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3.3364811267552003E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.12592303120589901</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.190772121010711</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.476789796956538</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.41011518602540697</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.99704982704570599</v>
+      </c>
+      <c r="J12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12">
+        <f>COUNTIF(C12:I12, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3.57243487563281E-2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.12987453183875999</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2.25538251358071E-4</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.17148617481932699</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.111164725190309</v>
+      </c>
+      <c r="H13" s="6">
+        <v>7.8839526340427499E-2</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.99264285324426305</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13">
+        <f>COUNTIF(C13:I13, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6">
+        <v>122</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.230678134287821</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.2873510856270499E-4</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.30641742956507501</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2.21756735353518E-5</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.52194018664113495</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.41665327932476898</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.99992048157246305</v>
+      </c>
+      <c r="J14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14">
+        <f>COUNTIF(C14:I14, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.28625167393078998</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.15690287149214199</v>
+      </c>
+      <c r="E15" s="6">
+        <v>7.9226404186952797E-3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1.2113305034984201E-3</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.476789796956538</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.41011518602540697</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.999961251174459</v>
+      </c>
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15">
+        <f>COUNTIF(C15:I15, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6">
+        <v>175</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.142297064581308</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2.05401741806788E-2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>9.5721294405232596E-2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.19782260918566799</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.71624201738654303</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.87283592461714499</v>
+      </c>
+      <c r="I16" s="7">
+        <v>8.5860051290964601E-9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <f>COUNTIF(C16:I16, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="6">
+        <v>92</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.49872361729854298</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.767675355057575</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.24089661690838901</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.35175360990337701</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1.01681984823847E-2</v>
+      </c>
+      <c r="H17" s="6">
+        <v>2.2438660844825601E-2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.99770119878975905</v>
+      </c>
+      <c r="J17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17">
+        <f>COUNTIF(C17:I17, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1039</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.95610461638608801</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.89806563115510696</v>
+      </c>
+      <c r="E18" s="6">
+        <v>8.5903454568038801E-2</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.87421532365325505</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1.10586504062926E-5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>6.4624680882641199E-5</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.21319451206333101</v>
+      </c>
+      <c r="J18" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18">
+        <f>COUNTIF(C18:I18, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" t="s">
+        <v>124</v>
+      </c>
+      <c r="N18" t="s">
+        <v>125</v>
+      </c>
+      <c r="O18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="6">
+        <v>56</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.34283661136059501</v>
+      </c>
+      <c r="D19" s="6">
+        <v>5.7592472000431903E-2</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.15426698075502199</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.23165840023697801</v>
+      </c>
+      <c r="G19" s="6">
+        <v>8.2880049322197093E-3</v>
+      </c>
+      <c r="H19" s="6">
+        <v>4.0643150653059098E-3</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.999996783231201</v>
+      </c>
+      <c r="J19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19">
+        <f>COUNTIF(C19:I19, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>245</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.27581267992089997</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.53829056640134698</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.521942509662638</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.68674971765378101</v>
+      </c>
+      <c r="G20" s="6">
+        <v>2.4480107499066799E-2</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.15788311947360201</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1.82005814102215E-5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20">
+        <f>COUNTIF(C20:I20, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="6">
+        <v>105</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.54549638605395601</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.81112119357250101</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.26999907614877899</v>
+      </c>
+      <c r="F21" s="6">
+        <v>8.6840811133584106E-2</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.18932391763919601</v>
+      </c>
+      <c r="H21" s="6">
+        <v>7.6344714444572803E-3</v>
+      </c>
+      <c r="I21" s="6">
+        <v>4.0765674222679397E-2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21">
+        <f>COUNTIF(C21:I21, "&lt;.05")</f>
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>109</v>
+      </c>
+      <c r="M21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="6">
+        <v>39</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3.4100868333172898E-2</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.46074947272298</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.110074023491538</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.167575015927836</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.106566504037604</v>
+      </c>
+      <c r="H22" s="6">
+        <v>7.5455980067085898E-2</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.96879355761847796</v>
+      </c>
+      <c r="J22" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22">
+        <f>COUNTIF(C22:I22, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="6">
+        <v>51</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.31768927784830098</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.190542383393286</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.14149638174449</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2.37887681736343E-2</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.16462151133264699</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0.450273054502843</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.96071607348235999</v>
+      </c>
+      <c r="J23" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23">
+        <f>COUNTIF(C23:I23, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="6">
+        <v>98</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.16577675648571</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.199270444209111</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.25446658519146498</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1.08884804099398E-2</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.75668306898114102</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0.31641141666281702</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.32415351289852001</v>
+      </c>
+      <c r="J24" t="s">
+        <v>105</v>
+      </c>
+      <c r="K24">
+        <f>COUNTIF(C24:I24, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="6">
+        <v>59</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.35748205966736002</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.236627944915099</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.16184012587654001</v>
+      </c>
+      <c r="F25" s="6">
+        <v>3.1171380596194599E-2</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.57246860574749003</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.15039409106142801</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.53946412336448002</v>
+      </c>
+      <c r="J25" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25">
+        <f>COUNTIF(C25:I25, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="6">
+        <v>62</v>
+      </c>
+      <c r="C26" s="6">
+        <v>7.8014297120865897E-2</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.25409037053188599</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.16934705750436499</v>
+      </c>
+      <c r="F26" s="6">
+        <v>3.4144569424255103E-2</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.22151059610332999</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0.16263090329983901</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0.99745345564964405</v>
+      </c>
+      <c r="J26" t="s">
+        <v>105</v>
+      </c>
+      <c r="K26">
+        <f>COUNTIF(C26:I26, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1797</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.179069767174799</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.141038537351345</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.159249309527181</v>
+      </c>
+      <c r="F27" s="6">
+        <v>3.1161291052372898E-3</v>
+      </c>
+      <c r="G27" s="6">
+        <v>5.1139277795045499E-2</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.34608093314094202</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.14337998222654599</v>
+      </c>
+      <c r="J27" t="s">
+        <v>105</v>
+      </c>
+      <c r="K27">
+        <f>COUNTIF(C27:I27, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="6">
+        <v>108</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.19247707538405601</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2.7570881254124199E-2</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.27655873697384198</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.39900250322828101</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.20022521843145899</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.71907087793797297</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0.99999999017849295</v>
+      </c>
+      <c r="J28" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28">
+        <f>COUNTIF(C28:I28, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6">
+        <v>200</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.187444003171155</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.206096362884544</v>
+      </c>
+      <c r="E29" s="6">
+        <v>2.1571483674723599E-2</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.240877413931783</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.54615436595252798</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0.67958652479898096</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0.999999835659381</v>
+      </c>
+      <c r="J29" t="s">
+        <v>107</v>
+      </c>
+      <c r="K29">
+        <f>COUNTIF(C29:I29, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>109</v>
+      </c>
+      <c r="M29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="6">
+        <v>120</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.59411455795950296</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.564391916495527</v>
+      </c>
+      <c r="E30" s="6">
+        <v>5.4345257525967297E-3</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.43219746944979698</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.51308854219945499</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.164312510928321</v>
+      </c>
+      <c r="I30" s="6">
+        <v>0.99999993650339702</v>
+      </c>
+      <c r="J30" t="s">
+        <v>107</v>
+      </c>
+      <c r="K30">
+        <f>COUNTIF(C30:I30, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="6">
+        <v>51</v>
+      </c>
+      <c r="C31" s="6">
+        <v>5.54127781625392E-2</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.554227179565425</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.14149638174449</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.21333231953078399</v>
+      </c>
+      <c r="G31" s="6">
+        <v>3.6138919079186503E-2</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.11882004324720399</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.99999002694988604</v>
+      </c>
+      <c r="J31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31">
+        <f>COUNTIF(C31:I31, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="6">
+        <v>61</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.36706561513069702</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.61966907026502205</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.16685206904803801</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0.24956387935157001</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.21625745640510799</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5.5216984320411999E-3</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0.944415545478692</v>
+      </c>
+      <c r="J32" t="s">
+        <v>85</v>
+      </c>
+      <c r="K32">
+        <f>COUNTIF(C32:I32, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="6">
+        <v>77</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.438806689792135</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.34107203331720298</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.20590812166341499</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.30414437103792202</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.30085297349845003</v>
+      </c>
+      <c r="H33" s="6">
+        <v>2.02461184930258E-3</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0.28152448570522598</v>
+      </c>
+      <c r="J33" t="s">
+        <v>85</v>
+      </c>
+      <c r="K33">
+        <f>COUNTIF(C33:I33, "&lt;.05")</f>
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>109</v>
+      </c>
+      <c r="M33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B35" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="6">
+        <v>105</v>
+      </c>
+      <c r="D35" s="6">
+        <v>220</v>
+      </c>
+      <c r="E35" s="6">
+        <v>42</v>
+      </c>
+      <c r="F35" s="6">
+        <v>66</v>
+      </c>
+      <c r="G35" s="6">
+        <v>200</v>
+      </c>
+      <c r="H35" s="6">
+        <v>164</v>
+      </c>
+      <c r="I35" s="6">
+        <v>2801</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K33">
+    <sortCondition descending="1" ref="K3:K33"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:I33">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+      <formula>0</formula>
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="6">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6">
+        <v>170</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6">
+        <v>113</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6">
+        <v>97</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1210</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="6">
+        <v>80</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="6">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="6">
+        <v>97</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6">
+        <v>122</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6">
+        <v>175</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="6">
+        <v>92</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1039</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="6">
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>245</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="6">
+        <v>105</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="6">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="6">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="6">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="6">
+        <v>59</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="6">
+        <v>62</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1797</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="6">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6">
+        <v>200</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="6">
+        <v>120</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="6">
+        <v>51</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="6">
+        <v>61</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="6">
+        <v>77</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="16" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q43" sqref="A1:Q43"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4635,1241 +6707,6 @@
     <sortCondition sortBy="cellColor" ref="Q3:Q62" dxfId="2"/>
   </sortState>
   <conditionalFormatting sqref="H1:K1 O1:Q1 O3:Q62 H3:K62">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
-      <formula>0</formula>
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
-    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="5">
-        <v>49</v>
-      </c>
-      <c r="C3" s="6">
-        <v>3.0727421786891403E-5</v>
-      </c>
-      <c r="D3" s="5">
-        <v>4.1408677795375499E-2</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1.31240589928971E-5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1.5519218270286801E-3</v>
-      </c>
-      <c r="G3" s="5">
-        <v>5.1642273572096702E-3</v>
-      </c>
-      <c r="H3" s="5">
-        <v>2.4966587012933399E-3</v>
-      </c>
-      <c r="I3" s="6">
-        <v>3.9374514759771299E-10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3">
-        <f>COUNTIF(C3:I3, "&lt;.05")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5">
-        <v>170</v>
-      </c>
-      <c r="C4" s="5">
-        <v>3.82764266623059E-2</v>
-      </c>
-      <c r="D4" s="5">
-        <v>5.1596458589716801E-2</v>
-      </c>
-      <c r="E4" s="5">
-        <v>9.1145456733761995E-2</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.189328930289766</v>
-      </c>
-      <c r="G4" s="5">
-        <v>3.0580940643272201E-3</v>
-      </c>
-      <c r="H4" s="5">
-        <v>4.8680620812544498E-2</v>
-      </c>
-      <c r="I4" s="5">
-        <v>4.1400693470308697E-2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4">
-        <f>COUNTIF(C4:I4, "&lt;.05")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="5">
-        <v>113</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1.00917630888977E-2</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3.2636679075339799E-2</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.28736385326993102</v>
-      </c>
-      <c r="F5" s="5">
-        <v>9.8320086435050205E-2</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.48127789556697198</v>
-      </c>
-      <c r="H5" s="5">
-        <v>4.2980989788245001E-2</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.25808089613206397</v>
-      </c>
-      <c r="J5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5">
-        <f>COUNTIF(C5:I5, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5">
-        <v>97</v>
-      </c>
-      <c r="C6" s="5">
-        <v>3.5842824028819401E-2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8.2715555596224498E-4</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.25222148564160102</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.36689888451437702</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.40408191903381802</v>
-      </c>
-      <c r="H6" s="5">
-        <v>2.66227001630235E-2</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.10749916758988599</v>
-      </c>
-      <c r="J6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K6">
-        <f>COUNTIF(C6:I6, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1210</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2.0028910919589501E-4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>4.4746813663012501E-3</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.14778188417742599</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.33807821000114202</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.56393306759295503</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.66049254676589397</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>93</v>
-      </c>
-      <c r="K7">
-        <f>COUNTIF(C7:I7, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="5">
-        <v>63</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.37650756713623701</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.25991936329413001</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1.5110016556087799E-2</v>
-      </c>
-      <c r="F8" s="5">
-        <v>3.5159386902263702E-2</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.596454664061291</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.52261680978378</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1.3409651500317901E-8</v>
-      </c>
-      <c r="J8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8">
-        <f>COUNTIF(C8:I8, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="5">
-        <v>80</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.119810503657902</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.71879934460762096</v>
-      </c>
-      <c r="E9" s="5">
-        <v>2.36831800814752E-2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>6.2428503719827999E-3</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.106283581417212</v>
-      </c>
-      <c r="H9" s="5">
-        <v>6.6532792544706995E-2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1.3999679440974699E-3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>94</v>
-      </c>
-      <c r="K9">
-        <f>COUNTIF(C9:I9, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="5">
-        <v>39</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0.25337999817992202</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.124610014084039</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.110074023491538</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1.43307083179275E-2</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.7944823064988499E-2</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1.06057084232558E-3</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0.38626838697876198</v>
-      </c>
-      <c r="J10" t="s">
-        <v>95</v>
-      </c>
-      <c r="K10">
-        <f>COUNTIF(C10:I10, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="5">
-        <v>97</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.51725204957717397</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.785452385130046</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.25222148564160102</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.36689888451437702</v>
-      </c>
-      <c r="G11" s="5">
-        <v>4.7136880600406899E-4</v>
-      </c>
-      <c r="H11" s="5">
-        <v>9.3785787513489495E-4</v>
-      </c>
-      <c r="I11" s="6">
-        <v>5.6903370904137798E-12</v>
-      </c>
-      <c r="J11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K11">
-        <f>COUNTIF(C11:I11, "&lt;.05")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="5">
-        <v>45</v>
-      </c>
-      <c r="C12" s="5">
-        <v>4.5505193561934396E-3</v>
-      </c>
-      <c r="D12" s="5">
-        <v>3.3364811267552003E-2</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.12592303120589901</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.190772121010711</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.476789796956538</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.41011518602540697</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.99704982704570599</v>
-      </c>
-      <c r="J12" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12">
-        <f>COUNTIF(C12:I12, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="5">
-        <v>40</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3.57243487563281E-2</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.12987453183875999</v>
-      </c>
-      <c r="E13" s="5">
-        <v>2.25538251358071E-4</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.17148617481932699</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.111164725190309</v>
-      </c>
-      <c r="H13" s="5">
-        <v>7.8839526340427499E-2</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.99264285324426305</v>
-      </c>
-      <c r="J13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K13">
-        <f>COUNTIF(C13:I13, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="5">
-        <v>122</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.230678134287821</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.2873510856270499E-4</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.30641742956507501</v>
-      </c>
-      <c r="F14" s="6">
-        <v>2.21756735353518E-5</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0.52194018664113495</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0.41665327932476898</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0.99992048157246305</v>
-      </c>
-      <c r="J14" t="s">
-        <v>99</v>
-      </c>
-      <c r="K14">
-        <f>COUNTIF(C14:I14, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="5">
-        <v>45</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.28625167393078998</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.15690287149214199</v>
-      </c>
-      <c r="E15" s="5">
-        <v>7.9226404186952797E-3</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1.2113305034984201E-3</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0.476789796956538</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0.41011518602540697</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0.999961251174459</v>
-      </c>
-      <c r="J15" t="s">
-        <v>100</v>
-      </c>
-      <c r="K15">
-        <f>COUNTIF(C15:I15, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="5">
-        <v>175</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0.142297064581308</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2.05401741806788E-2</v>
-      </c>
-      <c r="E16" s="5">
-        <v>9.5721294405232596E-2</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0.19782260918566799</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0.71624201738654303</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.87283592461714499</v>
-      </c>
-      <c r="I16" s="6">
-        <v>8.5860051290964601E-9</v>
-      </c>
-      <c r="J16" t="s">
-        <v>101</v>
-      </c>
-      <c r="K16">
-        <f>COUNTIF(C16:I16, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="5">
-        <v>92</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0.49872361729854298</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.767675355057575</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0.24089661690838901</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0.35175360990337701</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1.01681984823847E-2</v>
-      </c>
-      <c r="H17" s="5">
-        <v>2.2438660844825601E-2</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0.99770119878975905</v>
-      </c>
-      <c r="J17" t="s">
-        <v>102</v>
-      </c>
-      <c r="K17">
-        <f>COUNTIF(C17:I17, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1039</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0.95610461638608801</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.89806563115510696</v>
-      </c>
-      <c r="E18" s="5">
-        <v>8.5903454568038801E-2</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0.87421532365325505</v>
-      </c>
-      <c r="G18" s="6">
-        <v>1.10586504062926E-5</v>
-      </c>
-      <c r="H18" s="6">
-        <v>6.4624680882641199E-5</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0.21319451206333101</v>
-      </c>
-      <c r="J18" t="s">
-        <v>102</v>
-      </c>
-      <c r="K18">
-        <f>COUNTIF(C18:I18, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="5">
-        <v>56</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0.34283661136059501</v>
-      </c>
-      <c r="D19" s="5">
-        <v>5.7592472000431903E-2</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0.15426698075502199</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0.23165840023697801</v>
-      </c>
-      <c r="G19" s="5">
-        <v>8.2880049322197093E-3</v>
-      </c>
-      <c r="H19" s="5">
-        <v>4.0643150653059098E-3</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0.999996783231201</v>
-      </c>
-      <c r="J19" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19">
-        <f>COUNTIF(C19:I19, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5">
-        <v>245</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0.27581267992089997</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.53829056640134698</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0.521942509662638</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0.68674971765378101</v>
-      </c>
-      <c r="G20" s="5">
-        <v>2.4480107499066799E-2</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0.15788311947360201</v>
-      </c>
-      <c r="I20" s="6">
-        <v>1.82005814102215E-5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>103</v>
-      </c>
-      <c r="K20">
-        <f>COUNTIF(C20:I20, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="5">
-        <v>105</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0.54549638605395601</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.81112119357250101</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0.26999907614877899</v>
-      </c>
-      <c r="F21" s="5">
-        <v>8.6840811133584106E-2</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0.18932391763919601</v>
-      </c>
-      <c r="H21" s="5">
-        <v>7.6344714444572803E-3</v>
-      </c>
-      <c r="I21" s="5">
-        <v>4.0765674222679397E-2</v>
-      </c>
-      <c r="J21" t="s">
-        <v>104</v>
-      </c>
-      <c r="K21">
-        <f>COUNTIF(C21:I21, "&lt;.05")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="5">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5">
-        <v>3.4100868333172898E-2</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.46074947272298</v>
-      </c>
-      <c r="E22" s="5">
-        <v>0.110074023491538</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0.167575015927836</v>
-      </c>
-      <c r="G22" s="5">
-        <v>0.106566504037604</v>
-      </c>
-      <c r="H22" s="5">
-        <v>7.5455980067085898E-2</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0.96879355761847796</v>
-      </c>
-      <c r="J22" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22">
-        <f>COUNTIF(C22:I22, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="5">
-        <v>51</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0.31768927784830098</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0.190542383393286</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0.14149638174449</v>
-      </c>
-      <c r="F23" s="5">
-        <v>2.37887681736343E-2</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0.16462151133264699</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.450273054502843</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0.96071607348235999</v>
-      </c>
-      <c r="J23" t="s">
-        <v>106</v>
-      </c>
-      <c r="K23">
-        <f>COUNTIF(C23:I23, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="5">
-        <v>98</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0.16577675648571</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0.199270444209111</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0.25446658519146498</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1.08884804099398E-2</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0.75668306898114102</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0.31641141666281702</v>
-      </c>
-      <c r="I24" s="5">
-        <v>0.32415351289852001</v>
-      </c>
-      <c r="J24" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24">
-        <f>COUNTIF(C24:I24, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="5">
-        <v>59</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0.35748205966736002</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0.236627944915099</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0.16184012587654001</v>
-      </c>
-      <c r="F25" s="5">
-        <v>3.1171380596194599E-2</v>
-      </c>
-      <c r="G25" s="5">
-        <v>0.57246860574749003</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0.15039409106142801</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0.53946412336448002</v>
-      </c>
-      <c r="J25" t="s">
-        <v>106</v>
-      </c>
-      <c r="K25">
-        <f>COUNTIF(C25:I25, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="5">
-        <v>62</v>
-      </c>
-      <c r="C26" s="5">
-        <v>7.8014297120865897E-2</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0.25409037053188599</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0.16934705750436499</v>
-      </c>
-      <c r="F26" s="5">
-        <v>3.4144569424255103E-2</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0.22151059610332999</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0.16263090329983901</v>
-      </c>
-      <c r="I26" s="5">
-        <v>0.99745345564964405</v>
-      </c>
-      <c r="J26" t="s">
-        <v>106</v>
-      </c>
-      <c r="K26">
-        <f>COUNTIF(C26:I26, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="5">
-        <v>1797</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0.179069767174799</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0.141038537351345</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0.159249309527181</v>
-      </c>
-      <c r="F27" s="5">
-        <v>3.1161291052372898E-3</v>
-      </c>
-      <c r="G27" s="5">
-        <v>5.1139277795045499E-2</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0.34608093314094202</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0.14337998222654599</v>
-      </c>
-      <c r="J27" t="s">
-        <v>106</v>
-      </c>
-      <c r="K27">
-        <f>COUNTIF(C27:I27, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="5">
-        <v>108</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0.19247707538405601</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2.7570881254124199E-2</v>
-      </c>
-      <c r="E28" s="5">
-        <v>0.27655873697384198</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0.39900250322828101</v>
-      </c>
-      <c r="G28" s="5">
-        <v>0.20022521843145899</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0.71907087793797297</v>
-      </c>
-      <c r="I28" s="5">
-        <v>0.99999999017849295</v>
-      </c>
-      <c r="J28" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28">
-        <f>COUNTIF(C28:I28, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="5">
-        <v>200</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0.187444003171155</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0.206096362884544</v>
-      </c>
-      <c r="E29" s="5">
-        <v>2.1571483674723599E-2</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0.240877413931783</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0.54615436595252798</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0.67958652479898096</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0.999999835659381</v>
-      </c>
-      <c r="J29" t="s">
-        <v>108</v>
-      </c>
-      <c r="K29">
-        <f>COUNTIF(C29:I29, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="5">
-        <v>120</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0.59411455795950296</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0.564391916495527</v>
-      </c>
-      <c r="E30" s="5">
-        <v>5.4345257525967297E-3</v>
-      </c>
-      <c r="F30" s="5">
-        <v>0.43219746944979698</v>
-      </c>
-      <c r="G30" s="5">
-        <v>0.51308854219945499</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0.164312510928321</v>
-      </c>
-      <c r="I30" s="5">
-        <v>0.99999993650339702</v>
-      </c>
-      <c r="J30" t="s">
-        <v>108</v>
-      </c>
-      <c r="K30">
-        <f>COUNTIF(C30:I30, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="5">
-        <v>51</v>
-      </c>
-      <c r="C31" s="5">
-        <v>5.54127781625392E-2</v>
-      </c>
-      <c r="D31" s="5">
-        <v>0.554227179565425</v>
-      </c>
-      <c r="E31" s="5">
-        <v>0.14149638174449</v>
-      </c>
-      <c r="F31" s="5">
-        <v>0.21333231953078399</v>
-      </c>
-      <c r="G31" s="5">
-        <v>3.6138919079186503E-2</v>
-      </c>
-      <c r="H31" s="5">
-        <v>0.11882004324720399</v>
-      </c>
-      <c r="I31" s="5">
-        <v>0.99999002694988604</v>
-      </c>
-      <c r="J31" t="s">
-        <v>103</v>
-      </c>
-      <c r="K31">
-        <f>COUNTIF(C31:I31, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="5">
-        <v>61</v>
-      </c>
-      <c r="C32" s="5">
-        <v>0.36706561513069702</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0.61966907026502205</v>
-      </c>
-      <c r="E32" s="5">
-        <v>0.16685206904803801</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0.24956387935157001</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0.21625745640510799</v>
-      </c>
-      <c r="H32" s="5">
-        <v>5.5216984320411999E-3</v>
-      </c>
-      <c r="I32" s="5">
-        <v>0.944415545478692</v>
-      </c>
-      <c r="J32" t="s">
-        <v>85</v>
-      </c>
-      <c r="K32">
-        <f>COUNTIF(C32:I32, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="5">
-        <v>77</v>
-      </c>
-      <c r="C33" s="5">
-        <v>0.438806689792135</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0.34107203331720298</v>
-      </c>
-      <c r="E33" s="5">
-        <v>0.20590812166341499</v>
-      </c>
-      <c r="F33" s="5">
-        <v>0.30414437103792202</v>
-      </c>
-      <c r="G33" s="5">
-        <v>0.30085297349845003</v>
-      </c>
-      <c r="H33" s="5">
-        <v>2.02461184930258E-3</v>
-      </c>
-      <c r="I33" s="5">
-        <v>0.28152448570522598</v>
-      </c>
-      <c r="J33" t="s">
-        <v>85</v>
-      </c>
-      <c r="K33">
-        <f>COUNTIF(C33:I33, "&lt;.05")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B35" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="5">
-        <v>105</v>
-      </c>
-      <c r="D35" s="5">
-        <v>220</v>
-      </c>
-      <c r="E35" s="5">
-        <v>42</v>
-      </c>
-      <c r="F35" s="5">
-        <v>66</v>
-      </c>
-      <c r="G35" s="5">
-        <v>200</v>
-      </c>
-      <c r="H35" s="5">
-        <v>164</v>
-      </c>
-      <c r="I35" s="5">
-        <v>2801</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K33">
-    <sortCondition descending="1" ref="K3:K33"/>
-  </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:H1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C2:I33">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>0</formula>
       <formula>0.05</formula>

</xml_diff>